<commit_message>
Add USDA nutritions - WIP Fix copper attributes Add xls attribute table to git
</commit_message>
<xml_diff>
--- a/csvFiles/table_nutrition_attribute.xlsx
+++ b/csvFiles/table_nutrition_attribute.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShayMoshe\PycharmProjects\myFoodsNutrition\csvFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5B2CE4-BF02-45FD-B05D-DC56E3AB426B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8E9307-0B96-4BEA-AB09-C6F7E9DA78BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75226151-463E-4448-A347-206A7D11D3F3}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="195">
   <si>
     <t>nutritionUID</t>
   </si>
@@ -106,9 +106,6 @@
     <t>sugars</t>
   </si>
   <si>
-    <t>מתוכן סוכרים</t>
-  </si>
-  <si>
     <t>total_lipid_fat</t>
   </si>
   <si>
@@ -632,6 +629,9 @@
   </si>
   <si>
     <t>copper_cu</t>
+  </si>
+  <si>
+    <t>סוכרים</t>
   </si>
 </sst>
 </file>
@@ -735,9 +735,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -775,7 +775,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -881,7 +881,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1023,7 +1023,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EBCB2B-5690-40C1-8B8E-A4375CE6ED9D}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1083,8 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1910</v>
+        <f>1970*1.05</f>
+        <v>2068.5</v>
       </c>
       <c r="D2">
         <v>-1000</v>
@@ -1092,7 +1093,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -1110,7 +1111,8 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <f>0.25*C2/4</f>
+        <v>129.28125</v>
       </c>
       <c r="D3">
         <v>-1000</v>
@@ -1137,7 +1139,8 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>252</v>
+        <f>C2*0.45/4</f>
+        <v>232.70625000000001</v>
       </c>
       <c r="D4">
         <v>-1000</v>
@@ -1146,7 +1149,7 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -1173,10 +1176,10 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>194</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1188,22 +1191,23 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <f>C2*0.3/9</f>
+        <v>68.949999999999989</v>
+      </c>
+      <c r="D6">
+        <v>-1000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>-1000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1215,7 +1219,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1230,7 +1234,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1242,22 +1246,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>-1000</v>
+      </c>
+      <c r="E8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8">
-        <v>-1</v>
-      </c>
-      <c r="D8">
-        <v>-1000</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1269,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>1.5</v>
@@ -1278,13 +1282,13 @@
         <v>-1000</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1296,7 +1300,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>38</v>
@@ -1308,10 +1312,10 @@
         <v>13</v>
       </c>
       <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
         <v>31</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1323,7 +1327,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -1338,7 +1342,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1350,7 +1354,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>8.9999999999999998E-4</v>
@@ -1359,13 +1363,13 @@
         <v>-1000</v>
       </c>
       <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" t="s">
         <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" t="s">
-        <v>37</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1377,7 +1381,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1386,13 +1390,13 @@
         <v>-1000</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1404,7 +1408,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14">
         <v>1.1999999999999999E-3</v>
@@ -1413,13 +1417,13 @@
         <v>-1000</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1431,7 +1435,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>1.2999999999999999E-3</v>
@@ -1440,13 +1444,13 @@
         <v>-1000</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1458,7 +1462,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>1.6E-2</v>
@@ -1467,13 +1471,13 @@
         <v>-1000</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1485,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <v>0.55000000000000004</v>
@@ -1494,13 +1498,13 @@
         <v>-1000</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1512,7 +1516,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>5.0000000000000001E-3</v>
@@ -1521,13 +1525,13 @@
         <v>-1000</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1539,7 +1543,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19">
         <v>1.2999999999999999E-3</v>
@@ -1548,13 +1552,13 @@
         <v>-1000</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1566,7 +1570,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>3.0000000000000001E-5</v>
@@ -1575,13 +1579,13 @@
         <v>-1000</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1593,7 +1597,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21">
         <v>4.0000000000000002E-4</v>
@@ -1602,13 +1606,13 @@
         <v>-1000</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1620,7 +1624,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>2.3999999999999999E-6</v>
@@ -1629,13 +1633,13 @@
         <v>-1000</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -1647,7 +1651,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23">
         <v>0.09</v>
@@ -1656,13 +1660,13 @@
         <v>-1000</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1674,7 +1678,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24">
         <v>1.5E-5</v>
@@ -1683,13 +1687,13 @@
         <v>-1000</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1701,7 +1705,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25">
         <v>1.4999999999999999E-2</v>
@@ -1710,13 +1714,13 @@
         <v>-1000</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1728,7 +1732,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26">
         <v>1.2E-4</v>
@@ -1737,13 +1741,13 @@
         <v>-1000</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1755,22 +1759,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>-1000</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" t="s">
         <v>66</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>-1000</v>
-      </c>
-      <c r="E27" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" t="s">
-        <v>113</v>
-      </c>
-      <c r="G27" t="s">
-        <v>67</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1782,7 +1786,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28">
         <v>8.0000000000000002E-3</v>
@@ -1791,13 +1795,13 @@
         <v>-1000</v>
       </c>
       <c r="E28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1809,7 +1813,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29">
         <v>0.42</v>
@@ -1818,13 +1822,13 @@
         <v>-1000</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1836,7 +1840,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30">
         <v>0.7</v>
@@ -1845,13 +1849,13 @@
         <v>-1000</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -1863,7 +1867,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31">
         <v>1.0999999999999999E-2</v>
@@ -1872,13 +1876,13 @@
         <v>-1000</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1890,7 +1894,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>4.7</v>
@@ -1899,13 +1903,13 @@
         <v>-1000</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -1917,7 +1921,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33">
         <v>95.5</v>
@@ -1932,7 +1936,7 @@
         <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -1944,7 +1948,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C34">
         <v>1.6</v>
@@ -1956,10 +1960,10 @@
         <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1971,7 +1975,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C35">
         <v>17</v>
@@ -1983,10 +1987,10 @@
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -1998,7 +2002,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -2013,7 +2017,7 @@
         <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2025,7 +2029,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -2040,7 +2044,7 @@
         <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -2052,7 +2056,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38">
         <v>8.0000000000000002E-3</v>
@@ -2061,13 +2065,13 @@
         <v>-1000</v>
       </c>
       <c r="E38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F38" t="s">
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -2079,7 +2083,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39">
         <v>2.2999999999999998</v>
@@ -2094,7 +2098,7 @@
         <v>10</v>
       </c>
       <c r="G39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2106,7 +2110,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40">
         <v>3.4999999999999997E-5</v>
@@ -2115,13 +2119,13 @@
         <v>-1000</v>
       </c>
       <c r="E40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2133,7 +2137,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C41">
         <v>8.9999999999999998E-4</v>
@@ -2142,13 +2146,13 @@
         <v>-1000</v>
       </c>
       <c r="E41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2160,7 +2164,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42">
         <v>4.0000000000000001E-3</v>
@@ -2169,13 +2173,13 @@
         <v>-1000</v>
       </c>
       <c r="E42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F42" t="s">
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2187,7 +2191,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43">
         <v>1.4999999999999999E-4</v>
@@ -2196,13 +2200,13 @@
         <v>-1000</v>
       </c>
       <c r="E43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" t="s">
         <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -2214,7 +2218,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44">
         <v>2.3E-3</v>
@@ -2223,13 +2227,13 @@
         <v>-1000</v>
       </c>
       <c r="E44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" t="s">
         <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -2241,7 +2245,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45">
         <v>4.5000000000000003E-5</v>
@@ -2250,13 +2254,13 @@
         <v>-1000</v>
       </c>
       <c r="E45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -2268,7 +2272,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46">
         <v>5.5000000000000002E-5</v>
@@ -2277,13 +2281,13 @@
         <v>-1000</v>
       </c>
       <c r="E46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -2295,22 +2299,22 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47">
+        <v>-1</v>
+      </c>
+      <c r="D47">
+        <v>-1000</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
         <v>105</v>
       </c>
-      <c r="C47">
-        <v>-1</v>
-      </c>
-      <c r="D47">
-        <v>-1000</v>
-      </c>
-      <c r="E47" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>106</v>
-      </c>
-      <c r="G47" t="s">
-        <v>107</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -2322,19 +2326,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48">
+        <v>-1</v>
+      </c>
+      <c r="D48">
+        <v>-1000</v>
+      </c>
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" t="s">
         <v>108</v>
-      </c>
-      <c r="C48">
-        <v>-1</v>
-      </c>
-      <c r="D48">
-        <v>-1000</v>
-      </c>
-      <c r="E48" t="s">
-        <v>26</v>
-      </c>
-      <c r="G48" t="s">
-        <v>109</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -2346,19 +2350,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49">
+        <v>-1</v>
+      </c>
+      <c r="D49">
+        <v>-1000</v>
+      </c>
+      <c r="E49" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" t="s">
         <v>110</v>
-      </c>
-      <c r="C49">
-        <v>-1</v>
-      </c>
-      <c r="D49">
-        <v>-1000</v>
-      </c>
-      <c r="E49" t="s">
-        <v>26</v>
-      </c>
-      <c r="G49" t="s">
-        <v>111</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -2370,19 +2374,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50">
+        <v>-1</v>
+      </c>
+      <c r="D50">
+        <v>-1000</v>
+      </c>
+      <c r="E50" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" t="s">
         <v>122</v>
-      </c>
-      <c r="C50">
-        <v>-1</v>
-      </c>
-      <c r="D50">
-        <v>-1000</v>
-      </c>
-      <c r="E50" t="s">
-        <v>36</v>
-      </c>
-      <c r="G50" t="s">
-        <v>123</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -2394,19 +2398,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51">
+        <v>-1</v>
+      </c>
+      <c r="D51">
+        <v>-1000</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" t="s">
         <v>124</v>
-      </c>
-      <c r="C51">
-        <v>-1</v>
-      </c>
-      <c r="D51">
-        <v>-1000</v>
-      </c>
-      <c r="E51" t="s">
-        <v>36</v>
-      </c>
-      <c r="G51" t="s">
-        <v>125</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -2418,19 +2422,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52">
+        <v>-1</v>
+      </c>
+      <c r="D52">
+        <v>-1000</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" t="s">
         <v>127</v>
-      </c>
-      <c r="C52">
-        <v>-1</v>
-      </c>
-      <c r="D52">
-        <v>-1000</v>
-      </c>
-      <c r="E52" t="s">
-        <v>36</v>
-      </c>
-      <c r="G52" t="s">
-        <v>128</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -2442,22 +2446,22 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53">
+        <v>-1</v>
+      </c>
+      <c r="D53">
+        <v>-1000</v>
+      </c>
+      <c r="E53" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" t="s">
+        <v>128</v>
+      </c>
+      <c r="G53" t="s">
         <v>130</v>
-      </c>
-      <c r="C53">
-        <v>-1</v>
-      </c>
-      <c r="D53">
-        <v>-1000</v>
-      </c>
-      <c r="E53" t="s">
-        <v>36</v>
-      </c>
-      <c r="F53" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" t="s">
-        <v>131</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -2469,7 +2473,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54">
         <v>-1</v>
@@ -2478,10 +2482,10 @@
         <v>-1000</v>
       </c>
       <c r="E54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -2493,7 +2497,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C55">
         <v>-1</v>
@@ -2502,10 +2506,10 @@
         <v>-1000</v>
       </c>
       <c r="E55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -2517,7 +2521,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C56">
         <v>-1</v>
@@ -2526,10 +2530,10 @@
         <v>-1000</v>
       </c>
       <c r="E56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -2541,7 +2545,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C57">
         <v>-1</v>
@@ -2553,7 +2557,7 @@
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -2565,7 +2569,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -2577,7 +2581,7 @@
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -2589,7 +2593,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C59">
         <v>-1</v>
@@ -2601,7 +2605,7 @@
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2613,7 +2617,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C60">
         <v>-1</v>
@@ -2625,7 +2629,7 @@
         <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -2637,7 +2641,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C61">
         <v>-1</v>
@@ -2649,7 +2653,7 @@
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -2661,7 +2665,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C62">
         <v>-1</v>
@@ -2673,7 +2677,7 @@
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -2685,7 +2689,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C63">
         <v>-1</v>
@@ -2697,7 +2701,7 @@
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -2709,7 +2713,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C64">
         <v>-1</v>
@@ -2721,7 +2725,7 @@
         <v>13</v>
       </c>
       <c r="G64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -2733,7 +2737,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C65">
         <v>-1</v>
@@ -2745,7 +2749,7 @@
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -2757,7 +2761,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C66">
         <v>-1</v>
@@ -2769,7 +2773,7 @@
         <v>13</v>
       </c>
       <c r="G66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -2781,7 +2785,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C67">
         <v>-1</v>
@@ -2793,7 +2797,7 @@
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -2805,7 +2809,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C68">
         <v>-1</v>
@@ -2817,7 +2821,7 @@
         <v>13</v>
       </c>
       <c r="G68" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -2829,7 +2833,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C69">
         <v>-1</v>
@@ -2841,7 +2845,7 @@
         <v>13</v>
       </c>
       <c r="G69" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -2853,7 +2857,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C70">
         <v>-1</v>
@@ -2865,10 +2869,10 @@
         <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -2880,7 +2884,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C71">
         <v>-1</v>
@@ -2892,10 +2896,10 @@
         <v>13</v>
       </c>
       <c r="F71" t="s">
+        <v>164</v>
+      </c>
+      <c r="G71" t="s">
         <v>165</v>
-      </c>
-      <c r="G71" t="s">
-        <v>166</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -2907,7 +2911,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C72">
         <v>-1</v>
@@ -2919,7 +2923,7 @@
         <v>13</v>
       </c>
       <c r="G72" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -2931,7 +2935,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C73">
         <v>-1</v>
@@ -2943,10 +2947,10 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
+        <v>167</v>
+      </c>
+      <c r="G73" t="s">
         <v>168</v>
-      </c>
-      <c r="G73" t="s">
-        <v>169</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -2958,19 +2962,19 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74">
+        <v>-1</v>
+      </c>
+      <c r="D74">
+        <v>-1000</v>
+      </c>
+      <c r="E74" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" t="s">
         <v>170</v>
-      </c>
-      <c r="C74">
-        <v>-1</v>
-      </c>
-      <c r="D74">
-        <v>-1000</v>
-      </c>
-      <c r="E74" t="s">
-        <v>13</v>
-      </c>
-      <c r="G74" t="s">
-        <v>171</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -2982,19 +2986,19 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>171</v>
+      </c>
+      <c r="C75">
+        <v>-1</v>
+      </c>
+      <c r="D75">
+        <v>-1000</v>
+      </c>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" t="s">
         <v>172</v>
-      </c>
-      <c r="C75">
-        <v>-1</v>
-      </c>
-      <c r="D75">
-        <v>-1000</v>
-      </c>
-      <c r="E75" t="s">
-        <v>13</v>
-      </c>
-      <c r="G75" t="s">
-        <v>173</v>
       </c>
       <c r="H75">
         <v>0</v>

</xml_diff>